<commit_message>
update the time manage excle
</commit_message>
<xml_diff>
--- a/documents/IOS开发小组时间记录表.xlsx
+++ b/documents/IOS开发小组时间记录表.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="75" windowWidth="14295" windowHeight="6195" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="75" windowWidth="14295" windowHeight="6195" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="总计" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="21">
   <si>
     <t>日期</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -105,6 +105,24 @@
   <si>
     <t>学习游戏的菜单设计，完成：
 游戏暂停菜单和关卡选择菜单</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>2012.4.9</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>1.修改enemyball的运动方式函数，
+不同类型的球有不同的运行轨迹
+2.修改球的生命值与颜色变化。1-红、
+  2-橙、3-黄、4-绿、其他未白色。
+3.修改@property的习惯写法。@property成员变量名，变为_+名字</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>球的血量现在是以颜色辨别。
+为了不让颜色太多而使人眼花，
+现在暂定有5种颜色。</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -600,7 +618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B9" sqref="B8:B9"/>
     </sheetView>
   </sheetViews>
@@ -654,17 +672,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B6:B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="21.75" customWidth="1"/>
     <col min="2" max="2" width="33" customWidth="1"/>
-    <col min="3" max="3" width="24" customWidth="1"/>
+    <col min="3" max="3" width="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -712,6 +730,20 @@
       </c>
       <c r="D4">
         <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="81">
+      <c r="A5" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>